<commit_message>
Update of URL for species
</commit_message>
<xml_diff>
--- a/form_reporting_templates/Form-1RC.xlsx
+++ b/form_reporting_templates/Form-1RC.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\repositories\data_dissemination\iotc-reference-forms\form_reporting_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\repositories\data-reporting\iotc-reference-forms\form_reporting_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FAD312-6998-48BE-B450-81CFB2BC334C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F8A4CA-0912-420E-9927-076251F80989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="5O4euoXp3wZfikUhVbwGMfw3acpHwF0QGHqLGhqkSE4QfnoccY7VPEsDDzzEBP5NB49UT+XbcZf1lZQTbDpLFA==" workbookSaltValue="DtEOIJKZ9UKP8oWrD+QpRw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -258,7 +258,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -589,6 +589,30 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -602,7 +626,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -810,18 +834,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1824,7 +1838,7 @@
       <c r="DC4" s="71"/>
       <c r="DD4" s="71"/>
       <c r="DE4" s="71"/>
-      <c r="DF4" s="72"/>
+      <c r="DF4" s="71"/>
     </row>
     <row r="5" spans="1:110" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="35" t="s">
@@ -2606,7 +2620,7 @@
       <c r="J55" s="53"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="g2/Z765IujREFNzjMvM+R5OCGgOyKBAvIdVQJn2S1d6kfsFptg6Dp/KUO1J3imMZJMmrl4LYeQh/Sc+2VtX3Xw==" saltValue="8CfP7/MHo4SnPOGYKh14hA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="o/aMX/ctE+vE+3wwnBsLSp3jQR82RU8JgABtS9/SA1WckTSR/wNyQychBaXnf4BG3tOGHt0cp2lt5BgZXsneZg==" saltValue="O5OKEDbE8C45hfR0YqTPtA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="5">
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="I4:J4"/>
@@ -2626,20 +2640,15 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" location="fisheries" xr:uid="{ED342AB9-03F0-4794-A5E6-2197300C6DDA}"/>
-    <hyperlink ref="K4:DF4" r:id="rId2" location="allSpecies" display="Catch by species (live weight equivalent, t)" xr:uid="{6D429590-9E18-4205-80BE-F7414C6B378F}"/>
-    <hyperlink ref="I5" r:id="rId3" location="coverageTypes" xr:uid="{724F0376-2EAE-4203-9E7A-1897AD6BE90D}"/>
-    <hyperlink ref="H5" r:id="rId4" location="processingsRC" xr:uid="{5844FCEC-A2EF-428B-9D50-04D8BF8E519B}"/>
-    <hyperlink ref="G5" r:id="rId5" location="sourcesRC" xr:uid="{5E959ED6-0253-4C6D-BC73-58B2DECD8EF2}"/>
-    <hyperlink ref="F5" r:id="rId6" location="types" xr:uid="{2597D7D4-6064-4ED1-8FC4-B173B89E3472}"/>
-    <hyperlink ref="E5" r:id="rId7" location="retainReasons" xr:uid="{F3495450-D39C-4DF1-B164-52AAC0FEF034}"/>
-    <hyperlink ref="D5" r:id="rId8" location="IOTCareasMain" xr:uid="{63734AA0-E854-4685-861A-F679BE0AC281}"/>
-    <hyperlink ref="BD4:BM4" r:id="rId9" location="species" display="Catch by species (live weight equivalent, t)" xr:uid="{EB82D4FF-753B-4014-970A-379A57B589E3}"/>
-    <hyperlink ref="AT4:BC4" r:id="rId10" location="species" display="Catch by species (live weight equivalent, t)" xr:uid="{0A31174B-268F-4EB6-A38F-8B2A0B88DA3E}"/>
-    <hyperlink ref="AJ4:AS4" r:id="rId11" location="species" display="Catch by species (live weight equivalent, t)" xr:uid="{A38A1D9F-00CA-41AD-9F14-206078B78027}"/>
-    <hyperlink ref="Z4:AI4" r:id="rId12" location="species" display="Catch by species (live weight equivalent, t)" xr:uid="{7D67B08B-20D4-4621-A791-A9D4AC7454C0}"/>
-    <hyperlink ref="P4:Y4" r:id="rId13" location="species" display="Catch by species (live weight equivalent, t)" xr:uid="{678DEDB5-3D8A-4EA1-878F-4DD628D30BF9}"/>
+    <hyperlink ref="I5" r:id="rId2" location="coverageTypes" xr:uid="{724F0376-2EAE-4203-9E7A-1897AD6BE90D}"/>
+    <hyperlink ref="H5" r:id="rId3" location="processingsRC" xr:uid="{5844FCEC-A2EF-428B-9D50-04D8BF8E519B}"/>
+    <hyperlink ref="G5" r:id="rId4" location="sourcesRC" xr:uid="{5E959ED6-0253-4C6D-BC73-58B2DECD8EF2}"/>
+    <hyperlink ref="F5" r:id="rId5" location="types" xr:uid="{2597D7D4-6064-4ED1-8FC4-B173B89E3472}"/>
+    <hyperlink ref="E5" r:id="rId6" location="retainReasons" xr:uid="{F3495450-D39C-4DF1-B164-52AAC0FEF034}"/>
+    <hyperlink ref="D5" r:id="rId7" location="IOTCareasMain" xr:uid="{63734AA0-E854-4685-861A-F679BE0AC281}"/>
+    <hyperlink ref="K4:DF4" r:id="rId8" location="allSpecies" display="Catch by species (live weight equivalent, t)" xr:uid="{514550A4-1415-42DF-ABE7-7C5A4947C2BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>